<commit_message>
oh my gosh I cant spell
</commit_message>
<xml_diff>
--- a/docs/Homework/Tanzania_data.xlsx
+++ b/docs/Homework/Tanzania_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://calvincollege-my.sharepoint.com/personal/ena5_calvin_edu/Documents/Spring 2025/Data 304/Ella-Data304/docs/Homework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{A8A752BF-C9C7-4F01-998C-6FDA99C93C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E9DCDEB-DDE8-49F5-AACA-1E51A48089C4}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{A8A752BF-C9C7-4F01-998C-6FDA99C93C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ABE47DE-0F36-4B0D-8DA7-63B23D56F624}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BCC67C4B-63AB-4202-9239-E40CA187F57D}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>fertlity_rate</t>
-  </si>
-  <si>
     <t>contraception_use</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>1992-01-01</t>
+  </si>
+  <si>
+    <t>fertility_rate</t>
   </si>
 </sst>
 </file>
@@ -471,15 +471,15 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="11.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -490,21 +490,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>5.2</v>
@@ -521,7 +521,7 @@
         <v>2010</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>5.4</v>
@@ -535,10 +535,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
         <v>5.7</v>
@@ -555,7 +555,7 @@
         <v>1999</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>5.6</v>
@@ -572,7 +572,7 @@
         <v>1996</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
         <v>5.8</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
         <v>6.2</v>

</xml_diff>

<commit_message>
changed a variable name
</commit_message>
<xml_diff>
--- a/docs/Homework/Tanzania_data.xlsx
+++ b/docs/Homework/Tanzania_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://calvincollege-my.sharepoint.com/personal/ena5_calvin_edu/Documents/Spring 2025/Data 304/Ella-Data304/docs/Homework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{A8A752BF-C9C7-4F01-998C-6FDA99C93C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ABE47DE-0F36-4B0D-8DA7-63B23D56F624}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{A8A752BF-C9C7-4F01-998C-6FDA99C93C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60F025CE-A3AC-4E2E-88E4-D3F10A45DAF6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BCC67C4B-63AB-4202-9239-E40CA187F57D}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>contraception_use</t>
   </si>
   <si>
-    <t>fam_plan_need</t>
-  </si>
-  <si>
     <t>2015-2016</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>fertility_rate</t>
+  </si>
+  <si>
+    <t>fam_plan_unmet</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +479,7 @@
     <col min="1" max="2" width="11.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -490,21 +490,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>5.2</v>
@@ -521,7 +521,7 @@
         <v>2010</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>5.4</v>
@@ -535,10 +535,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>5.7</v>
@@ -555,7 +555,7 @@
         <v>1999</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>5.6</v>
@@ -572,7 +572,7 @@
         <v>1996</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>5.8</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1">
         <v>6.2</v>

</xml_diff>